<commit_message>
discussion part 2 and proofreading checks
</commit_message>
<xml_diff>
--- a/figures/gradient_table_formatted.xlsx
+++ b/figures/gradient_table_formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PalaeoClimateGradient\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{518D5EB2-51B6-43EB-91A6-7DA3BBE569BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68EE915-EC6E-489C-97D1-333328BB7CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5580" windowWidth="29040" windowHeight="15840" xr2:uid="{E9044DC6-30D8-4EE5-B81E-60FB352BBD1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9044DC6-30D8-4EE5-B81E-60FB352BBD1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Source</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Gaussian function</t>
   </si>
   <si>
-    <t>Bij et al. (2009)</t>
-  </si>
-  <si>
     <t>Keating-Bitoni et al. (2011)</t>
   </si>
   <si>
@@ -463,6 +460,12 @@
   </si>
   <si>
     <t>none (model simulations)</t>
+  </si>
+  <si>
+    <t>tropics - deep water</t>
+  </si>
+  <si>
+    <t>Bijl et al. (2009)</t>
   </si>
 </sst>
 </file>
@@ -915,7 +918,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
@@ -968,10 +971,10 @@
     </row>
     <row r="2" spans="1:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>7</v>
@@ -980,10 +983,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -1006,7 +1009,7 @@
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -1018,10 +1021,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -1044,10 +1047,10 @@
     </row>
     <row r="4" spans="1:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>12</v>
@@ -1059,7 +1062,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -1082,13 +1085,13 @@
     </row>
     <row r="5" spans="1:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -1097,7 +1100,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -1120,22 +1123,22 @@
     </row>
     <row r="6" spans="1:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -1158,10 +1161,10 @@
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="11">
         <v>26</v>
@@ -1170,10 +1173,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>

</xml_diff>

<commit_message>
manuscript and cover letter updates
</commit_message>
<xml_diff>
--- a/figures/gradient_table_formatted.xlsx
+++ b/figures/gradient_table_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PalaeoClimateGradient\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68EE915-EC6E-489C-97D1-333328BB7CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA2FE2-BADD-49BF-A7F5-20BE1FC74D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9044DC6-30D8-4EE5-B81E-60FB352BBD1F}"/>
   </bookViews>
@@ -453,19 +453,19 @@
     </r>
   </si>
   <si>
-    <t>climate model ensemble</t>
-  </si>
-  <si>
     <t>Pross et al. 2012, as shown in Tierney et al. (2017)</t>
   </si>
   <si>
-    <t>none (model simulations)</t>
-  </si>
-  <si>
     <t>tropics - deep water</t>
   </si>
   <si>
     <t>Bijl et al. (2009)</t>
+  </si>
+  <si>
+    <t>climate model ensemble (GCM)</t>
+  </si>
+  <si>
+    <t>none (GCM simulations)</t>
   </si>
 </sst>
 </file>
@@ -918,7 +918,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +971,7 @@
     </row>
     <row r="2" spans="1:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
@@ -1132,7 +1132,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>5</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="7" spans="1:24" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>14</v>
@@ -1173,10 +1173,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>

</xml_diff>